<commit_message>
Making broadcast weights more dynamic
</commit_message>
<xml_diff>
--- a/Testing/TestingPhase2.xlsx
+++ b/Testing/TestingPhase2.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nina/Downloads/W2021 TO DO/MSCI 435/msci435-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nina/Downloads/W2021 TO DO/MSCI 435/msci435-project/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{020CE59B-12C1-C647-B35F-D192A5D133D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE22DD1-7633-FF4A-B8C4-CA538400A0C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="2" xr2:uid="{F4BB75D5-A56C-3B48-B8D2-08E9FB93149A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="5" xr2:uid="{F4BB75D5-A56C-3B48-B8D2-08E9FB93149A}"/>
   </bookViews>
   <sheets>
     <sheet name="Con 3 &lt;=" sheetId="1" r:id="rId1"/>
     <sheet name="All Con - 24h" sheetId="2" r:id="rId2"/>
     <sheet name="All Con - 24h - 2" sheetId="3" r:id="rId3"/>
-    <sheet name="No Con 1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="No Con 1" sheetId="4" r:id="rId5"/>
+    <sheet name="Final Results" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="46">
   <si>
     <t>1-fl</t>
   </si>
@@ -164,12 +166,24 @@
   <si>
     <t>24</t>
   </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Nina's Improvements from model</t>
+  </si>
+  <si>
+    <t>Reduces back and forth between judes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,8 +191,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +231,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0B7EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA186E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1C3DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE86CB6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -218,62 +288,257 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -286,6 +551,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE86CB6"/>
+      <color rgb="FFF1C3DE"/>
+      <color rgb="FFA186E9"/>
+      <color rgb="FFC0B7EE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -994,7 +1267,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:G15 A2:B15 I2:K15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2075,7 +2348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCCC92B-1676-094B-BA26-2557EB96A68F}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -3141,6 +3414,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952DEF6-8969-7C4A-AFCD-FCC0E0AD29F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E4BA4F-6E9B-DD48-BDA1-FA36007B6220}">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -3611,4 +3896,646 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C062F53-3DAB-B14E-99F1-6175CE9DC49B}">
+  <dimension ref="B2:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32">
+        <v>10</v>
+      </c>
+      <c r="I4" s="33">
+        <v>8</v>
+      </c>
+      <c r="J4" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="35">
+        <v>10</v>
+      </c>
+      <c r="H5" s="36">
+        <v>9</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="37">
+        <v>7</v>
+      </c>
+      <c r="H6" s="38">
+        <v>11</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="15">
+        <v>6</v>
+      </c>
+      <c r="G7" s="39">
+        <v>9</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="16">
+        <v>4</v>
+      </c>
+      <c r="G8" s="40">
+        <v>11</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="17">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="38">
+        <v>11</v>
+      </c>
+      <c r="J9" s="41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="20">
+        <v>2</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="42">
+        <v>7</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="18">
+        <v>5</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="44">
+        <v>8</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="21">
+        <v>6</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="45">
+        <v>12</v>
+      </c>
+      <c r="I12" s="36">
+        <v>9</v>
+      </c>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="23">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="42">
+        <v>7</v>
+      </c>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="25">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12">
+        <v>4</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="45">
+        <v>12</v>
+      </c>
+      <c r="J15" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="26">
+        <v>6</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="48">
+        <v>12</v>
+      </c>
+      <c r="H16" s="49">
+        <v>8</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="27">
+        <v>5</v>
+      </c>
+      <c r="D17" s="28">
+        <v>6</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30">
+        <v>1</v>
+      </c>
+      <c r="G17" s="51"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="52">
+        <v>10</v>
+      </c>
+      <c r="J17" s="53"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="24">
+        <v>3</v>
+      </c>
+      <c r="F22" s="66">
+        <v>5</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="67">
+        <v>10</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12">
+        <v>4</v>
+      </c>
+      <c r="F23" s="13">
+        <v>3</v>
+      </c>
+      <c r="G23" s="35">
+        <v>10</v>
+      </c>
+      <c r="H23" s="36">
+        <v>9</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="18">
+        <v>5</v>
+      </c>
+      <c r="F24" s="14">
+        <v>2</v>
+      </c>
+      <c r="G24" s="37">
+        <v>7</v>
+      </c>
+      <c r="H24" s="38">
+        <v>11</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="20">
+        <v>2</v>
+      </c>
+      <c r="F25" s="15">
+        <v>6</v>
+      </c>
+      <c r="G25" s="39">
+        <v>9</v>
+      </c>
+      <c r="H25" s="49">
+        <v>8</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="22">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
+        <v>4</v>
+      </c>
+      <c r="G26" s="40">
+        <v>11</v>
+      </c>
+      <c r="H26" s="42">
+        <v>7</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="26">
+        <v>6</v>
+      </c>
+      <c r="F27" s="68">
+        <v>1</v>
+      </c>
+      <c r="G27" s="44">
+        <v>8</v>
+      </c>
+      <c r="H27" s="45">
+        <v>12</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="48">
+        <v>12</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="17">
+        <v>2</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="21">
+        <v>6</v>
+      </c>
+      <c r="D30" s="22">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="49">
+        <v>8</v>
+      </c>
+      <c r="J30" s="69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
+      <c r="D31" s="24">
+        <v>3</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="38">
+        <v>11</v>
+      </c>
+      <c r="J31" s="46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="61">
+        <v>4</v>
+      </c>
+      <c r="D32" s="18">
+        <v>5</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="42">
+        <v>7</v>
+      </c>
+      <c r="J32" s="50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="25">
+        <v>3</v>
+      </c>
+      <c r="D33" s="20">
+        <v>2</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="45">
+        <v>12</v>
+      </c>
+      <c r="J33" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="62">
+        <v>5</v>
+      </c>
+      <c r="D34" s="12">
+        <v>4</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="36">
+        <v>9</v>
+      </c>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="51"/>
+      <c r="D35" s="28">
+        <v>6</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="52">
+        <v>10</v>
+      </c>
+      <c r="J35" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add broadcast channels & print obj fn value
</commit_message>
<xml_diff>
--- a/Testing/TestingPhase2.xlsx
+++ b/Testing/TestingPhase2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nina/Downloads/W2021 TO DO/MSCI 435/msci435-project/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE22DD1-7633-FF4A-B8C4-CA538400A0C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D91835-8C9D-0642-9614-843ADA6AF487}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="5" xr2:uid="{F4BB75D5-A56C-3B48-B8D2-08E9FB93149A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="50">
   <si>
     <t>1-fl</t>
   </si>
@@ -176,7 +176,19 @@
     <t>Nina's Improvements from model</t>
   </si>
   <si>
-    <t>Reduces back and forth between judes</t>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Vault</t>
+  </si>
+  <si>
+    <t>Bars</t>
+  </si>
+  <si>
+    <t>Beam</t>
+  </si>
+  <si>
+    <t>Reduces back and forth between judges</t>
   </si>
 </sst>
 </file>
@@ -461,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -534,6 +546,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2349,7 +2366,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3900,20 +3917,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C062F53-3DAB-B14E-99F1-6175CE9DC49B}">
-  <dimension ref="B2:L35"/>
+  <dimension ref="B2:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="60" t="s">
         <v>42</v>
       </c>
@@ -3941,8 +3965,21 @@
       <c r="J3" s="56" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L3" s="76"/>
+      <c r="M3" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="58" t="s">
         <v>18</v>
       </c>
@@ -3968,8 +4005,17 @@
       <c r="J4" s="34">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="72">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M4" s="31">
+        <v>1</v>
+      </c>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="75"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="58" t="s">
         <v>19</v>
       </c>
@@ -3989,8 +4035,17 @@
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L5" s="72">
+        <v>0.375</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="58" t="s">
         <v>20</v>
       </c>
@@ -4008,8 +4063,17 @@
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="19"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L6" s="72">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="58" t="s">
         <v>21</v>
       </c>
@@ -4025,8 +4089,17 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L7" s="72">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="58" t="s">
         <v>22</v>
       </c>
@@ -4042,8 +4115,17 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L8" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="10">
+        <v>1</v>
+      </c>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="58" t="s">
         <v>23</v>
       </c>
@@ -4063,8 +4145,17 @@
       <c r="J9" s="41">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L9" s="72">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="58" t="s">
         <v>24</v>
       </c>
@@ -4082,8 +4173,17 @@
       <c r="J10" s="43">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L10" s="72">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11">
+        <v>1</v>
+      </c>
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="58" t="s">
         <v>25</v>
       </c>
@@ -4099,8 +4199,17 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L11" s="72">
+        <v>0.625</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1</v>
+      </c>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="58" t="s">
         <v>26</v>
       </c>
@@ -4120,8 +4229,17 @@
         <v>9</v>
       </c>
       <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L12" s="72">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M12" s="10">
+        <v>1</v>
+      </c>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="58" t="s">
         <v>27</v>
       </c>
@@ -4139,8 +4257,17 @@
       <c r="J13" s="46">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L13" s="72">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="M13" s="10">
+        <v>1</v>
+      </c>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="58" t="s">
         <v>28</v>
       </c>
@@ -4154,8 +4281,17 @@
         <v>7</v>
       </c>
       <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L14" s="72">
+        <v>0.75</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11">
+        <v>1</v>
+      </c>
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="58" t="s">
         <v>29</v>
       </c>
@@ -4177,8 +4313,17 @@
       <c r="J15" s="47">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L15" s="72">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M15" s="10">
+        <v>1</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="19"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="58" t="s">
         <v>30</v>
       </c>
@@ -4198,8 +4343,17 @@
       <c r="J16" s="50">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="72">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M16" s="10">
+        <v>1</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="59" t="s">
         <v>31</v>
       </c>
@@ -4219,13 +4373,22 @@
         <v>10</v>
       </c>
       <c r="J17" s="53"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="73">
+        <v>0.875</v>
+      </c>
+      <c r="M17" s="51">
+        <v>1</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="53"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="70" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="57" t="s">
         <v>42</v>
       </c>
@@ -4253,11 +4416,11 @@
       <c r="J21" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="71" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K21" s="71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="58" t="s">
         <v>18</v>
       </c>
@@ -4276,7 +4439,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="19"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="58" t="s">
         <v>19</v>
       </c>
@@ -4297,7 +4460,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="19"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="58" t="s">
         <v>20</v>
       </c>
@@ -4318,7 +4481,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="19"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="58" t="s">
         <v>21</v>
       </c>
@@ -4339,7 +4502,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="19"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="58" t="s">
         <v>22</v>
       </c>
@@ -4360,7 +4523,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="19"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="58" t="s">
         <v>23</v>
       </c>
@@ -4381,7 +4544,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="19"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="58" t="s">
         <v>24</v>
       </c>
@@ -4398,7 +4561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="58" t="s">
         <v>25</v>
       </c>
@@ -4415,7 +4578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="58" t="s">
         <v>26</v>
       </c>
@@ -4436,7 +4599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="58" t="s">
         <v>27</v>
       </c>
@@ -4457,7 +4620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="58" t="s">
         <v>28</v>
       </c>

</xml_diff>